<commit_message>
Fix discharge type mismatch
</commit_message>
<xml_diff>
--- a/mockup_data/mockup_data.xlsx
+++ b/mockup_data/mockup_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawarit\Desktop\GitHub\Foster-Ulcer-AI\Foster-Ulcer-AI\mockup_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FD4910-9AF8-46F8-923A-8B9D1486A597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E58C3D8-D8C0-4332-8AF9-DCA3A0917841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -4192,8 +4192,8 @@
   </sheetPr>
   <dimension ref="B2:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4787,7 +4787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8AA9DF-84AD-4C5A-B6B1-F52447F2C2E1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>